<commit_message>
Uploaded Final copy of HOWLERS (Lunar Madness) Project Tracking Sheet.xlsx to Resources Directory ~RS 1-27-25 @ 10:33pm
</commit_message>
<xml_diff>
--- a/Resources/HOWLERS (Lunar Madness) Project Tracking Sheet.xlsx
+++ b/Resources/HOWLERS (Lunar Madness) Project Tracking Sheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="74">
   <si>
     <t>Team Member</t>
   </si>
@@ -134,10 +134,10 @@
     <t xml:space="preserve">Review and provide feedback on all deliverables </t>
   </si>
   <si>
-    <t xml:space="preserve">Refine 6-8 required visualizations </t>
+    <t xml:space="preserve">Create / Refine 6-8 visualizations </t>
   </si>
   <si>
-    <t>Outstanding</t>
+    <t>Incomplete</t>
   </si>
   <si>
     <t>Review &amp; Assist if needed on presentation slides</t>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Ensure all requirements are met</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Final quality checks</t>
@@ -195,9 +192,6 @@
   </si>
   <si>
     <t xml:space="preserve">GitHub README file includes detailed usage and installation instructions </t>
-  </si>
-  <si>
-    <t>InProgress</t>
   </si>
   <si>
     <t>GitHub README includes either examples of the application, or the results and a summary of the analysis</t>
@@ -1824,7 +1818,7 @@
         <v>45682.0</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -1854,13 +1848,13 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="7">
         <v>45682.0</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -30886,19 +30880,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
@@ -30927,19 +30921,19 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="19"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="20">
         <v>2.0</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>27</v>
@@ -30947,13 +30941,13 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="20">
         <v>3.0</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>27</v>
@@ -30961,13 +30955,13 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="20">
         <v>2.0</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>27</v>
@@ -30975,13 +30969,13 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="20">
         <v>3.0</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>27</v>
@@ -30993,19 +30987,19 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="19"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="20">
         <v>3.0</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>27</v>
@@ -31013,13 +31007,13 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="20">
         <v>2.0</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>27</v>
@@ -31027,27 +31021,27 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="20">
         <v>2.0</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>56</v>
+      <c r="C12" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="20">
         <v>3.0</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>27</v>
@@ -31058,19 +31052,19 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="19"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="20">
         <v>10.0</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>27</v>
@@ -31078,13 +31072,13 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="20">
         <v>10.0</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>27</v>
@@ -31092,13 +31086,13 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="20">
         <v>5.0</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>27</v>
@@ -31106,19 +31100,19 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="19"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" s="20">
         <v>5.0</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>27</v>
@@ -31130,19 +31124,19 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" s="19"/>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" s="20">
         <v>10.0</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>27</v>
@@ -31150,13 +31144,13 @@
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="20">
         <v>5.0</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="22" t="s">
         <v>27</v>
@@ -31164,13 +31158,13 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B25" s="20">
         <v>5.0</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="22" t="s">
         <v>27</v>
@@ -31182,19 +31176,19 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B27" s="19"/>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B28" s="20">
         <v>5.0</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>27</v>
@@ -31202,13 +31196,13 @@
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" s="20">
         <v>5.0</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>27</v>
@@ -31216,13 +31210,13 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="20">
         <v>5.0</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>27</v>
@@ -31230,13 +31224,13 @@
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="20">
         <v>5.0</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="22" t="s">
         <v>27</v>
@@ -31244,13 +31238,13 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B32" s="20">
         <v>5.0</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>27</v>
@@ -31258,13 +31252,13 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="20">
         <v>3.0</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="22" t="s">
         <v>27</v>
@@ -31272,13 +31266,13 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B34" s="20">
         <v>2.0</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>27</v>

</xml_diff>